<commit_message>
a ton of work on website data
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb132/raw/Table20.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb132/raw/Table20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/wc_cc_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb132/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C61AEE-8F63-4141-8255-95AE9047B618}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000254F2-347B-EE47-89B3-E72536F1EBF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22460" yWindow="460" windowWidth="17000" windowHeight="26500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -572,7 +572,7 @@
   <dimension ref="A1:D90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1562,7 +1562,7 @@
         <v>7</v>
       </c>
       <c r="B72" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C72" s="2">
         <v>8928</v>

</xml_diff>